<commit_message>
BBL Half way ast vs DH
</commit_message>
<xml_diff>
--- a/Records/Stats - BBL 2024.xlsx
+++ b/Records/Stats - BBL 2024.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sachin\Personal\Cricket\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3F892-BC26-4179-96CF-0855153977DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449E473-2C66-4451-A189-5AE083C8EECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{82D476CB-B89A-4841-80AF-E4E5663C9360}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{82D476CB-B89A-4841-80AF-E4E5663C9360}"/>
   </bookViews>
   <sheets>
     <sheet name="C-BATTING" sheetId="6" r:id="rId1"/>
     <sheet name="C-BOWLING" sheetId="7" r:id="rId2"/>
+    <sheet name="Stats-Batting" sheetId="8" r:id="rId3"/>
+    <sheet name="Stats - Bowling" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'C-BOWLING'!$A$15:$D$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Stats - Bowling'!$A$1:$M$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Stats-Batting'!$A$1:$D$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="86">
   <si>
     <t>Runs</t>
   </si>
@@ -64,8 +68,209 @@
     <t>Wickets</t>
   </si>
   <si>
+    <t>BBL'24 - TOP BATSMAN</t>
+  </si>
+  <si>
+    <t>Naved A</t>
+  </si>
+  <si>
+    <t>Shrihari M</t>
+  </si>
+  <si>
+    <t>Nikhil J</t>
+  </si>
+  <si>
+    <t>Sandip S</t>
+  </si>
+  <si>
+    <t>Jeet S</t>
+  </si>
+  <si>
+    <t>Dinakar K</t>
+  </si>
+  <si>
+    <t>Manish K</t>
+  </si>
+  <si>
+    <t>BBL '24 - TOP BOWLER</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>total_match</t>
+  </si>
+  <si>
+    <t>total_wickets</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>Venkat G</t>
+  </si>
+  <si>
+    <t>Sikanderbasha R</t>
+  </si>
+  <si>
+    <t>Dinakar Krishnamurthy</t>
+  </si>
+  <si>
+    <t>Jeet Sidhu</t>
+  </si>
+  <si>
+    <t>Sandip Shingte</t>
+  </si>
+  <si>
+    <t>Sachien Mittal</t>
+  </si>
+  <si>
+    <t>Rajesh Pasupuleti</t>
+  </si>
+  <si>
+    <t>Nikhil Joy</t>
+  </si>
+  <si>
+    <t>Manish Kutar</t>
+  </si>
+  <si>
+    <t>Ramashish Singh</t>
+  </si>
+  <si>
+    <t>Avinash Krishnamurthy</t>
+  </si>
+  <si>
+    <t>Vivek P</t>
+  </si>
+  <si>
+    <t>Ud Khandelwal (udit)</t>
+  </si>
+  <si>
+    <t>Omer</t>
+  </si>
+  <si>
+    <t>Muthu Gurusamy</t>
+  </si>
+  <si>
+    <t>Deebak Chandar T</t>
+  </si>
+  <si>
+    <t>Dheeraj Kumar</t>
+  </si>
+  <si>
+    <t>Bharath Jayaraman</t>
+  </si>
+  <si>
+    <t>Rohit Koul</t>
+  </si>
+  <si>
+    <t>Khwaja Asif</t>
+  </si>
+  <si>
+    <t>Mandeep Jagotra</t>
+  </si>
+  <si>
+    <t>Siddharth Sharma</t>
+  </si>
+  <si>
+    <t>Ajith Sundaraj</t>
+  </si>
+  <si>
+    <t>Parag Deshpande</t>
+  </si>
+  <si>
+    <t>Ravindranath Reddy</t>
+  </si>
+  <si>
+    <t>Vineet Saxena</t>
+  </si>
+  <si>
+    <t>Sidh Singh</t>
+  </si>
+  <si>
+    <t>Kamlesh Malviya</t>
+  </si>
+  <si>
+    <t>Santhosh Kumar</t>
+  </si>
+  <si>
+    <t>Anand Gupta</t>
+  </si>
+  <si>
+    <t>Yogesh Maheshwari</t>
+  </si>
+  <si>
+    <t>Shrihari Mahale</t>
+  </si>
+  <si>
+    <t>Balachandar Pandian</t>
+  </si>
+  <si>
+    <t>Sudeep Dhed</t>
+  </si>
+  <si>
+    <t>Sasikumar Vinjam</t>
+  </si>
+  <si>
+    <t>Prasad Deosarkar</t>
+  </si>
+  <si>
+    <t>Naved A Alvi</t>
+  </si>
+  <si>
+    <t>Raman Prabhu</t>
+  </si>
+  <si>
+    <t>Gaurav Verma</t>
+  </si>
+  <si>
+    <t>Abhishek Dolas</t>
+  </si>
+  <si>
+    <t>Mohan Sivakumar</t>
+  </si>
+  <si>
+    <t>Ravi Shankar Pullagura</t>
+  </si>
+  <si>
+    <t>Dhaval</t>
+  </si>
+  <si>
+    <t>Naman Madan</t>
+  </si>
+  <si>
+    <t>Selva Ganesh B</t>
+  </si>
+  <si>
+    <t>Rajeev Kumar Sharma</t>
+  </si>
+  <si>
+    <t>Jai Balaji</t>
+  </si>
+  <si>
+    <t>Shubhavrato Roy</t>
+  </si>
+  <si>
+    <t>Jay Gangireddygari</t>
+  </si>
+  <si>
+    <t>Jairaj</t>
+  </si>
+  <si>
+    <t>Prakas Kannan</t>
+  </si>
+  <si>
+    <t>Abhijeet Tale</t>
+  </si>
+  <si>
+    <t>total_runs</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Highest Run Getter: ROHIT K </t>
+      <t xml:space="preserve">Highest Run Getter: Selva Ganesh </t>
     </r>
     <r>
       <rPr>
@@ -76,15 +281,21 @@
         <rFont val="Tw Cen MT"/>
         <family val="2"/>
       </rPr>
-      <t>(119)</t>
+      <t>(98)</t>
     </r>
   </si>
   <si>
-    <t>GOOGLY CUP '23 - TOP BOWLER</t>
+    <t>Qualifying MATCHES:- 2/10</t>
+  </si>
+  <si>
+    <t>Qualifying RUNS:- 40/200</t>
+  </si>
+  <si>
+    <t>Qualifying WICKETS:- 3/15</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Highest Wicket Taker: MUTHU G </t>
+      <t xml:space="preserve">Highest Wicket Taker: Venkat G </t>
     </r>
     <r>
       <rPr>
@@ -95,20 +306,26 @@
         <rFont val="Tw Cen MT"/>
         <family val="2"/>
       </rPr>
-      <t>(12)</t>
+      <t>(6)</t>
     </r>
   </si>
   <si>
-    <t>BBL'24 - TOP BATSMAN</t>
+    <t>Selva G</t>
   </si>
   <si>
-    <t>Qualifying MATCHES:- 0/20</t>
+    <t>Tasdid Hossain</t>
   </si>
   <si>
-    <t>Qualifying RUNS:- 0/200</t>
+    <t>Murali Krish</t>
   </si>
   <si>
-    <t>Qualifying WICKETS:- 8/30</t>
+    <t>Sambhaji Warang</t>
+  </si>
+  <si>
+    <t>Godavarthi Manikanta</t>
+  </si>
+  <si>
+    <t>Vijay Nagarajan</t>
   </si>
 </sst>
 </file>
@@ -118,7 +335,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -171,11 +388,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF4D4D4F"/>
-      <name val="Karla"/>
-    </font>
-    <font>
       <b/>
       <sz val="22"/>
       <color rgb="FFFFD700"/>
@@ -206,44 +418,29 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFEFEF"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD3D3D3"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFD3D3D3"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFD3D3D3"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFD3D3D3"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -312,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -320,41 +517,34 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -641,19 +831,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-</c:v>
+                  <c:v>Selva G</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-</c:v>
+                  <c:v>Nikhil J</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-</c:v>
+                  <c:v>Naved A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-</c:v>
+                  <c:v>Shrihari M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-</c:v>
+                  <c:v>Dinakar K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -665,19 +855,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,19 +1065,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-</c:v>
+                  <c:v>Selva G</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-</c:v>
+                  <c:v>Nikhil J</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-</c:v>
+                  <c:v>Naved A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-</c:v>
+                  <c:v>Shrihari M</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-</c:v>
+                  <c:v>Dinakar K</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1325,19 +1515,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-</c:v>
+                  <c:v>Sandip S</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-</c:v>
+                  <c:v>Jeet S</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-</c:v>
+                  <c:v>Manish K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-</c:v>
+                  <c:v>Dinakar K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-</c:v>
+                  <c:v>Venkat G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1349,19 +1539,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,19 +1749,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-</c:v>
+                  <c:v>Sandip S</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-</c:v>
+                  <c:v>Jeet S</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-</c:v>
+                  <c:v>Manish K</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-</c:v>
+                  <c:v>Dinakar K</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-</c:v>
+                  <c:v>Venkat G</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3016,7 +3206,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>49</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -3379,7 +3569,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Dinakar K</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -3470,7 +3660,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Shrihari M</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -3561,7 +3751,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Naved A</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -3652,7 +3842,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Nikhil J</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -3743,7 +3933,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Selva G</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -3843,7 +4033,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>43.5</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -3943,7 +4133,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>37.5</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -4043,7 +4233,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>24</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -4143,7 +4333,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>17.67</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -4225,7 +4415,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -4304,7 +4494,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>98</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
@@ -4378,7 +4568,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>3</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -4455,7 +4645,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -4532,7 +4722,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -4609,7 +4799,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>3</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -4688,7 +4878,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>87</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
@@ -4764,7 +4954,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>48</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
@@ -4840,7 +5030,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>75</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
@@ -4916,7 +5106,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>53</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
@@ -5119,16 +5309,13 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="800" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Verdana"/>
-            </a:rPr>
-            <a:t>Wicekts</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="800" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5138,14 +5325,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>643559</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>107673</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>77066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>671140</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>77066</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5159,9 +5346,9 @@
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6644309" y="917298"/>
-          <a:ext cx="713381" cy="131318"/>
+        <a:xfrm flipV="1">
+          <a:off x="6789255" y="1236631"/>
+          <a:ext cx="715037" cy="461304"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5189,16 +5376,13 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="800" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Verdana"/>
-            </a:rPr>
-            <a:t>Wicekts</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="800" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Tw Cen MT" panose="020B0602020104020603" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5397,7 +5581,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>7</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -5760,7 +5944,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Venkat G</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -5851,7 +6035,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Dinakar K</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -5942,7 +6126,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Manish K</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -6033,7 +6217,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Jeet S</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -6124,7 +6308,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>-</a:t>
+            <a:t>Sandip S</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1">
             <a:solidFill>
@@ -6224,7 +6408,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>7.75</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -6324,7 +6508,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>9</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -6424,7 +6608,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>9.25</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -6524,7 +6708,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="l"/>
-            <a:t>0.00</a:t>
+            <a:t>9.5</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -6606,7 +6790,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -6686,7 +6870,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>4</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -6764,7 +6948,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>3</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -6842,7 +7026,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>2</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -6920,7 +7104,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>3</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -6998,7 +7182,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>4</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7078,7 +7262,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>4</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7158,7 +7342,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>3</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7238,7 +7422,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>4</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7318,7 +7502,7 @@
               <a:ea typeface="Verdana"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>0</a:t>
+            <a:t>6</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7840,10 +8024,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E4D43C-FDA6-4CF6-A592-01D63194DCAA}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7853,382 +8038,390 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+    </row>
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <f>ROUND((B4/($B$6)),2)</f>
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:F3" si="0">ROUND((C4/($B$6)),2)</f>
+        <v>0.89</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+    </row>
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>43.5</v>
+      </c>
+      <c r="D4">
+        <v>37.5</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <f>MAX('Stats-Batting'!D:D)</f>
+        <v>49</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="e">
-        <f>ROUND((B4/($B$6)),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="10" t="e">
-        <f t="shared" ref="C3:F3" si="0">ROUND((C4/($B$6)),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D3" s="10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12">
-        <v>0</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="W8" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
+      <c r="B9">
+        <v>98</v>
+      </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9">
+        <v>48</v>
+      </c>
+      <c r="F9">
+        <v>53</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="W9" s="16"/>
+      <c r="I9" s="12"/>
+      <c r="W9" s="12"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="I10" s="16"/>
-      <c r="W10" s="16"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="I10" s="12"/>
+      <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I11" s="16"/>
-      <c r="W11" s="16"/>
+      <c r="I11" s="12"/>
+      <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I12" s="16"/>
-      <c r="W12" s="16"/>
+      <c r="I12" s="12"/>
+      <c r="W12" s="12"/>
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I13" s="16"/>
-      <c r="W13" s="16"/>
+      <c r="I13" s="12"/>
+      <c r="W13" s="12"/>
       <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I14" s="16"/>
-      <c r="W14" s="16"/>
+      <c r="I14" s="12"/>
+      <c r="W14" s="12"/>
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I15" s="16"/>
-      <c r="W15" s="16"/>
+      <c r="I15" s="12"/>
+      <c r="W15" s="12"/>
       <c r="Y15" s="3"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I16" s="16"/>
-      <c r="W16" s="16"/>
+      <c r="I16" s="12"/>
+      <c r="W16" s="12"/>
       <c r="Y16" s="3"/>
     </row>
     <row r="17" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I17" s="16"/>
-      <c r="W17" s="16"/>
+      <c r="I17" s="12"/>
+      <c r="W17" s="12"/>
     </row>
     <row r="18" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I18" s="16"/>
-      <c r="W18" s="16"/>
+      <c r="I18" s="12"/>
+      <c r="W18" s="12"/>
     </row>
     <row r="19" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I19" s="16"/>
-      <c r="W19" s="16"/>
+      <c r="I19" s="12"/>
+      <c r="W19" s="12"/>
     </row>
     <row r="20" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I20" s="16"/>
-      <c r="W20" s="16"/>
+      <c r="I20" s="12"/>
+      <c r="W20" s="12"/>
     </row>
     <row r="21" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I21" s="16"/>
-      <c r="W21" s="16"/>
+      <c r="I21" s="12"/>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I22" s="16"/>
-      <c r="W22" s="16"/>
+      <c r="I22" s="12"/>
+      <c r="W22" s="12"/>
     </row>
     <row r="23" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I23" s="16"/>
-      <c r="W23" s="16"/>
+      <c r="I23" s="12"/>
+      <c r="W23" s="12"/>
     </row>
     <row r="24" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I24" s="16"/>
-      <c r="W24" s="16"/>
+      <c r="I24" s="12"/>
+      <c r="W24" s="12"/>
     </row>
     <row r="25" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I25" s="16"/>
-      <c r="W25" s="16"/>
+      <c r="I25" s="12"/>
+      <c r="W25" s="12"/>
     </row>
     <row r="26" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I26" s="16"/>
-      <c r="W26" s="16"/>
+      <c r="I26" s="12"/>
+      <c r="W26" s="12"/>
     </row>
     <row r="27" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I27" s="16"/>
-      <c r="W27" s="16"/>
+      <c r="I27" s="12"/>
+      <c r="W27" s="12"/>
     </row>
     <row r="28" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="16"/>
-      <c r="W28" s="16"/>
+      <c r="I28" s="12"/>
+      <c r="W28" s="12"/>
     </row>
     <row r="29" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I29" s="16"/>
-      <c r="W29" s="16"/>
+      <c r="I29" s="12"/>
+      <c r="W29" s="12"/>
     </row>
     <row r="30" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I30" s="16"/>
-      <c r="W30" s="16"/>
+      <c r="I30" s="12"/>
+      <c r="W30" s="12"/>
     </row>
     <row r="31" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I31" s="16"/>
-      <c r="W31" s="16"/>
+      <c r="I31" s="12"/>
+      <c r="W31" s="12"/>
     </row>
     <row r="32" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I32" s="16"/>
-      <c r="W32" s="16"/>
+      <c r="I32" s="12"/>
+      <c r="W32" s="12"/>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I33" s="16"/>
-      <c r="W33" s="16"/>
+      <c r="I33" s="12"/>
+      <c r="W33" s="12"/>
     </row>
     <row r="34" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="16"/>
-      <c r="W34" s="16"/>
+      <c r="I34" s="12"/>
+      <c r="W34" s="12"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
     </row>
     <row r="37" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
     </row>
     <row r="39" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J39" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="19"/>
+      <c r="J39" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="15"/>
     </row>
     <row r="40" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J40" s="20"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-      <c r="V40" s="22"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="K2:U4"/>
     <mergeCell ref="J36:V37"/>
     <mergeCell ref="I8:I34"/>
     <mergeCell ref="W8:W34"/>
     <mergeCell ref="J39:V40"/>
+    <mergeCell ref="J2:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8238,10 +8431,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6406DA6A-BE7D-42D1-BCCC-700E27DB771C}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8252,23 +8446,23 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -8287,86 +8481,92 @@
       <c r="F2" s="5">
         <v>0.01</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+    </row>
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="e">
+      <c r="B3" s="6">
         <f>ROUND((B4/$B$6),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="6" t="e">
+        <v>0.13</v>
+      </c>
+      <c r="C3" s="6">
         <f t="shared" ref="C3:F3" si="0">ROUND((C4/$B$6),2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D3" s="6" t="e">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D3" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E3" s="6" t="e">
+        <v>0.16</v>
+      </c>
+      <c r="E3" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="6" t="e">
+        <v>0.17</v>
+      </c>
+      <c r="F3" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0.17</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+    </row>
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>7.75</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>9.25</v>
+      </c>
+      <c r="F4">
+        <v>9.5</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
@@ -8376,12 +8576,13 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>0</v>
+        <f>MAX('Stats - Bowling'!D:D)</f>
+        <v>55</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -8395,12 +8596,12 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="I7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="W7" s="16" t="s">
-        <v>14</v>
+      <c r="I7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="W7" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
@@ -8408,61 +8609,61 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="23"/>
-      <c r="W8" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="20"/>
+      <c r="W8" s="12"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="23"/>
-      <c r="W9" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="20"/>
+      <c r="W9" s="12"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I10" s="16"/>
-      <c r="J10" s="23"/>
-      <c r="W10" s="16"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="20"/>
+      <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I11" s="16"/>
-      <c r="J11" s="23"/>
-      <c r="W11" s="16"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="20"/>
+      <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I12" s="16"/>
-      <c r="J12" s="23"/>
-      <c r="W12" s="16"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="20"/>
+      <c r="W12" s="12"/>
       <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -8471,9 +8672,9 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="23"/>
-      <c r="W13" s="16"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="20"/>
+      <c r="W13" s="12"/>
       <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -8482,9 +8683,9 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="23"/>
-      <c r="W14" s="16"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="20"/>
+      <c r="W14" s="12"/>
       <c r="Y14" s="3"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -8493,9 +8694,9 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="23"/>
-      <c r="W15" s="16"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="20"/>
+      <c r="W15" s="12"/>
       <c r="Y15" s="3"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
@@ -8504,9 +8705,9 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="23"/>
-      <c r="W16" s="16"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="20"/>
+      <c r="W16" s="12"/>
       <c r="Y16" s="3"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -8515,9 +8716,9 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="23"/>
-      <c r="W17" s="16"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="20"/>
+      <c r="W17" s="12"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -8525,9 +8726,9 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="23"/>
-      <c r="W18" s="16"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="20"/>
+      <c r="W18" s="12"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -8535,9 +8736,9 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="23"/>
-      <c r="W19" s="16"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="20"/>
+      <c r="W19" s="12"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
@@ -8545,9 +8746,9 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="23"/>
-      <c r="W20" s="16"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="20"/>
+      <c r="W20" s="12"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
@@ -8555,9 +8756,9 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="23"/>
-      <c r="W21" s="16"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="20"/>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -8565,9 +8766,9 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="23"/>
-      <c r="W22" s="16"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="20"/>
+      <c r="W22" s="12"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
@@ -8575,9 +8776,9 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="23"/>
-      <c r="W23" s="16"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="20"/>
+      <c r="W23" s="12"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
@@ -8585,9 +8786,9 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="23"/>
-      <c r="W24" s="16"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="20"/>
+      <c r="W24" s="12"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
@@ -8595,9 +8796,9 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="23"/>
-      <c r="W25" s="16"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="20"/>
+      <c r="W25" s="12"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
@@ -8605,9 +8806,9 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="23"/>
-      <c r="W26" s="16"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="20"/>
+      <c r="W26" s="12"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
@@ -8615,9 +8816,9 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="23"/>
-      <c r="W27" s="16"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="20"/>
+      <c r="W27" s="12"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
@@ -8625,9 +8826,9 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="23"/>
-      <c r="W28" s="16"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="20"/>
+      <c r="W28" s="12"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
@@ -8635,9 +8836,9 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="23"/>
-      <c r="W29" s="16"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="20"/>
+      <c r="W29" s="12"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
@@ -8647,97 +8848,97 @@
       <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="23"/>
-      <c r="W30" s="16"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="20"/>
+      <c r="W30" s="12"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="I31" s="16"/>
-      <c r="J31" s="23"/>
-      <c r="W31" s="16"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="20"/>
+      <c r="W31" s="12"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="I32" s="16"/>
-      <c r="J32" s="23"/>
-      <c r="W32" s="16"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="20"/>
+      <c r="W32" s="12"/>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="I33" s="16"/>
-      <c r="J33" s="23"/>
-      <c r="W33" s="16"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="20"/>
+      <c r="W33" s="12"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
     </row>
     <row r="37" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
     </row>
     <row r="39" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J39" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="19"/>
+      <c r="J39" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="15"/>
     </row>
     <row r="40" spans="9:23" x14ac:dyDescent="0.2">
-      <c r="J40" s="20"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-      <c r="V40" s="22"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="18"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:D19">
     <sortCondition descending="1" ref="D16:D19"/>
   </sortState>
   <mergeCells count="6">
+    <mergeCell ref="J2:V4"/>
+    <mergeCell ref="I7:I33"/>
     <mergeCell ref="J39:V40"/>
-    <mergeCell ref="K2:U4"/>
     <mergeCell ref="J36:V37"/>
     <mergeCell ref="W7:W33"/>
-    <mergeCell ref="I7:I33"/>
     <mergeCell ref="J7:J33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8746,6 +8947,1619 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853278B2-E997-4E65-A0F2-3B0D296458F8}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>109</v>
+      </c>
+      <c r="D2">
+        <v>36.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>98</v>
+      </c>
+      <c r="D3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>87</v>
+      </c>
+      <c r="D4">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>73</v>
+      </c>
+      <c r="D5">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>17.670000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>39</v>
+      </c>
+      <c r="D11">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>26</v>
+      </c>
+      <c r="D19">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+      <c r="D27">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
+    <sortCondition descending="1" ref="D2:D54"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41456C1E-1B53-4A8C-84F0-3B1A93D11C8D}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:D58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>10.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>10.57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>9.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>11.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>23.67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M11">
+    <sortCondition ref="K2:K11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>